<commit_message>
add column to power automate
</commit_message>
<xml_diff>
--- a/PowerAutomate/Bank_Customers.xlsx
+++ b/PowerAutomate/Bank_Customers.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanlu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanlu\git\test_db\PowerAutomate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2649BC78-4A4D-4FC9-B26C-2132BC8ED2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EB42BA-85ED-43C8-89E7-91582BF3090A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$F$1:$F$21</definedName>
     <definedName name="query" localSheetId="0" hidden="1">data!$A$1:$E$21</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -23,15 +24,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\tanlu\Downloads\query.iqy" keepAlive="1" name="query" type="5" refreshedVersion="8" minRefreshableVersion="3" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" odcFile="C:\Users\tanlu\Downloads\query.iqy" keepAlive="1" name="query" type="5" refreshedVersion="8" minRefreshableVersion="3" saveData="1">
     <dbPr connection="Provider=Microsoft.Office.List.OLEDB.2.0;Data Source=&quot;&quot;;ApplicationName=Excel;Version=12.0.0.0" command="&lt;LIST&gt;&lt;VIEWGUID&gt;E7857967-8865-4ECA-83ED-248BD47D7646&lt;/VIEWGUID&gt;&lt;LISTNAME&gt;8ee64513-6a2c-4b9b-8f99-a489347b7312&lt;/LISTNAME&gt;&lt;LISTWEB&gt;https://mailkmuttacth.sharepoint.com/sites/DataAnalytics/_vti_bin&lt;/LISTWEB&gt;&lt;LISTSUBWEB&gt;&lt;/LISTSUBWEB&gt;&lt;ROOTFOLDER&gt;&lt;/ROOTFOLDER&gt;&lt;/LIST&gt;" commandType="5"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t>Customer ID</t>
   </si>
@@ -226,12 +227,18 @@
   </si>
   <si>
     <t>Cornish</t>
+  </si>
+  <si>
+    <t>Approval</t>
+  </si>
+  <si>
+    <t>Approved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -386,7 +393,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,8 +573,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -682,6 +701,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -727,10 +798,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -776,25 +856,163 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -810,14 +1028,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="query" backgroundRefresh="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="8">
-    <queryTableFields count="5">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="query" backgroundRefresh="0" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh nextId="9" unboundColumnsRight="1">
+    <queryTableFields count="6">
       <queryTableField id="1" name="Customer ID" tableColumnId="1"/>
       <queryTableField id="2" name="Name" tableColumnId="2"/>
       <queryTableField id="3" name="Surname" tableColumnId="3"/>
       <queryTableField id="4" name="Gender" tableColumnId="4"/>
       <queryTableField id="5" name="Age" tableColumnId="5"/>
+      <queryTableField id="8" dataBound="0" tableColumnId="6"/>
     </queryTableFields>
     <queryTableDeletedFields count="2">
       <deletedField name="Path"/>
@@ -828,17 +1047,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_query" displayName="Table_query" ref="A1:E21" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_query" displayName="Table_query" ref="A1:F21" tableType="queryTable" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:F21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E21">
     <sortCondition ref="A1:A21"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" uniqueName="Title" name="Customer ID" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" uniqueName="field_1" name="Name" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="3" uniqueName="field_2" name="Surname" queryTableFieldId="3" dataDxfId="2"/>
-    <tableColumn id="4" uniqueName="field_3" name="Gender" queryTableFieldId="4" dataDxfId="1"/>
-    <tableColumn id="5" uniqueName="field_4" name="Age" queryTableFieldId="5" dataDxfId="0"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="Title" name="Customer ID" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="field_1" name="Name" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="field_2" name="Surname" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="field_3" name="Gender" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="field_4" name="Age" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{83F27FBB-74F6-48ED-A47B-931120D0BBEA}" uniqueName="6" name="Approval" queryTableFieldId="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1140,11 +1360,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1154,363 +1374,427 @@
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
+      <c r="F2" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
+      <c r="F3" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
+      <c r="F4" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
+      <c r="F5" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
+      <c r="F6" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
+      <c r="F7" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
+      <c r="F8" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
+      <c r="F9" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
+      <c r="F10" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
+      <c r="F11" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
+      <c r="F12" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
+      <c r="F13" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
+      <c r="F14" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="s">
+      <c r="F15" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="s">
+      <c r="F16" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
+      <c r="F17" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
+      <c r="F18" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
+      <c r="F19" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
+      <c r="F20" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>31</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>